<commit_message>
add function implementation status to the decompose problem table
</commit_message>
<xml_diff>
--- a/references/decompose_problem.xlsx
+++ b/references/decompose_problem.xlsx
@@ -5,9 +5,14 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet 2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet 3" sheetId="3" r:id="rId6"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - Table 1" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet 1 - starry_ user inputs" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet 1 - jaxoplanet implementa" sheetId="4" r:id="rId7"/>
+    <sheet name="Sheet 2 - starry MathType" sheetId="5" r:id="rId8"/>
+    <sheet name="Sheet 2 - starry.math._get_cova" sheetId="6" r:id="rId9"/>
+    <sheet name="Sheet 2 - Drawings" sheetId="7" r:id="rId10"/>
+    <sheet name="Sheet 3" sheetId="8" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
@@ -18,7 +23,7 @@
     <author>dot</author>
   </authors>
   <commentList>
-    <comment ref="E17" authorId="0">
+    <comment ref="E16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -36,11 +41,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="203">
+  <si>
+    <t>This document was exported from Numbers. Each table was converted to an Excel spreadsheet. All other objects on each Numbers sheet were placed on separate work sheets. Please be aware that formula calculations may differ in Excel.</t>
+  </si>
+  <si>
+    <t>Numbers Sheet Name</t>
+  </si>
+  <si>
+    <t>Numbers Table Name</t>
+  </si>
+  <si>
+    <t>Excel Spreadsheet Name</t>
+  </si>
+  <si>
+    <t>Sheet 1</t>
+  </si>
   <si>
     <t>Table 1</t>
   </si>
   <si>
+    <t>Sheet 1 - Table 1</t>
+  </si>
+  <si>
     <t>science</t>
   </si>
   <si>
@@ -72,6 +95,9 @@
   </si>
   <si>
     <t>jaxoplanet function</t>
+  </si>
+  <si>
+    <t>status* (see code definition on the side table)</t>
   </si>
   <si>
     <t>Comment</t>
@@ -106,6 +132,9 @@
     <t xml:space="preserve">change-of-basis matrix: Ylms to polynomials </t>
   </si>
   <si>
+    <t>IM_1, T_4</t>
+  </si>
+  <si>
     <t>Eq. 53</t>
   </si>
   <si>
@@ -149,6 +178,9 @@
   </si>
   <si>
     <t>change-of-basis matrix: Ylms to Green’s polynomials</t>
+  </si>
+  <si>
+    <t>IM_1, T_2A</t>
   </si>
   <si>
     <t>get rotational phase curve</t>
@@ -193,6 +225,20 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
+      <t>rT_solution_vector</t>
+    </r>
+  </si>
+  <si>
+    <t>IM_3, T_2A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
       <t>R</t>
     </r>
   </si>
@@ -209,6 +255,9 @@
       </rPr>
       <t>R_full</t>
     </r>
+  </si>
+  <si>
+    <t>IM_2, T_4</t>
   </si>
   <si>
     <r>
@@ -278,6 +327,9 @@
     </r>
   </si>
   <si>
+    <t>IM_3, T_1</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u val="single"/>
@@ -292,9 +344,6 @@
     <t>R’: rotation matrix by an angle along z-axis</t>
   </si>
   <si>
-    <t>transform frame</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <u val="single"/>
@@ -306,6 +355,9 @@
     </r>
   </si>
   <si>
+    <t>transform frame</t>
+  </si>
+  <si>
     <t>M, inc, obl, theta</t>
   </si>
   <si>
@@ -318,6 +370,20 @@
       </rPr>
       <t>core.OpsYlm.right_project</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>right_project</t>
+    </r>
+  </si>
+  <si>
+    <t>IM_1, T_1</t>
   </si>
   <si>
     <r>
@@ -854,6 +920,9 @@
     <t>starry: user inputs</t>
   </si>
   <si>
+    <t>Sheet 1 - starry_ user inputs</t>
+  </si>
+  <si>
     <t xml:space="preserve">parameter </t>
   </si>
   <si>
@@ -863,9 +932,108 @@
     <t>optional true</t>
   </si>
   <si>
+    <t>jaxoplanet implementation: status</t>
+  </si>
+  <si>
+    <t>Sheet 1 - jaxoplanet implementa</t>
+  </si>
+  <si>
+    <t>function implementation</t>
+  </si>
+  <si>
+    <t>unit test</t>
+  </si>
+  <si>
+    <t>integration test</t>
+  </si>
+  <si>
+    <t>code (impl)</t>
+  </si>
+  <si>
+    <t>impl: non-jax (e.g. numpy)</t>
+  </si>
+  <si>
+    <t>impl: jax</t>
+  </si>
+  <si>
+    <t>impl: jax.jit</t>
+  </si>
+  <si>
+    <t>impl: optimization attempted</t>
+  </si>
+  <si>
+    <t>code (test)</t>
+  </si>
+  <si>
+    <t>test: compare with starry (minimal)</t>
+  </si>
+  <si>
+    <t>test: sympy (minimal)</t>
+  </si>
+  <si>
+    <t>test: compare with starry (larger parameter space)</t>
+  </si>
+  <si>
+    <t>test: sympy (larger parameter space)</t>
+  </si>
+  <si>
+    <t>code (verification)</t>
+  </si>
+  <si>
+    <t>verified with integration test</t>
+  </si>
+  <si>
+    <t>verified with integration test (jax.jit, numpyro?)</t>
+  </si>
+  <si>
+    <t>IM_1</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>T_1</t>
+  </si>
+  <si>
+    <t>V_1</t>
+  </si>
+  <si>
+    <t>IM_2</t>
+  </si>
+  <si>
+    <t>T_2A</t>
+  </si>
+  <si>
+    <t>V_2</t>
+  </si>
+  <si>
+    <t>IM_3</t>
+  </si>
+  <si>
+    <t>T_2B</t>
+  </si>
+  <si>
+    <t>IM_4</t>
+  </si>
+  <si>
+    <t>T_3A</t>
+  </si>
+  <si>
+    <t>T_3B</t>
+  </si>
+  <si>
+    <t>T_4</t>
+  </si>
+  <si>
+    <t>Sheet 2</t>
+  </si>
+  <si>
     <t>starry MathType</t>
   </si>
   <si>
+    <t>Sheet 2 - starry MathType</t>
+  </si>
+  <si>
     <t>scipy/numpy functions</t>
   </si>
   <si>
@@ -930,6 +1098,9 @@
   </si>
   <si>
     <t>starry.math._get_covariance</t>
+  </si>
+  <si>
+    <t>Sheet 2 - starry.math._get_cova</t>
   </si>
   <si>
     <t>required functions</t>
@@ -976,6 +1147,15 @@
   <si>
     <t>np.eye, np.sum, etc.</t>
   </si>
+  <si>
+    <t>“All Drawings from the Sheet”</t>
+  </si>
+  <si>
+    <t>Sheet 2 - Drawings</t>
+  </si>
+  <si>
+    <t>Sheet 3</t>
+  </si>
 </sst>
 </file>
 
@@ -984,7 +1164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -996,21 +1176,32 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="11"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="13"/>
-      <color indexed="9"/>
+      <color indexed="12"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b val="1"/>
       <sz val="22"/>
-      <color indexed="9"/>
+      <color indexed="12"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b val="1"/>
       <sz val="10"/>
-      <color indexed="9"/>
+      <color indexed="12"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -1019,15 +1210,15 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="9"/>
-      <name val="Helvetica Neue Medium"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Helvetica Neue Medium"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1036,7 +1227,7 @@
     </font>
     <font>
       <sz val="13"/>
-      <color indexed="9"/>
+      <color indexed="12"/>
       <name val="Helvetica Neue Medium"/>
     </font>
     <font>
@@ -1052,12 +1243,12 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="25"/>
+      <color indexed="29"/>
       <name val="Helvetica Neue Medium"/>
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="23"/>
+      <color indexed="27"/>
       <name val="Helvetica Neue Medium"/>
     </font>
     <font>
@@ -1067,7 +1258,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1076,37 +1267,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="18"/>
+        <fgColor indexed="16"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="19"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="20"/>
+        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -1134,6 +1319,30 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="25"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="28"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -1145,361 +1354,361 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="19"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="19"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="19"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="19"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="19"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="19"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1509,9 +1718,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -1519,268 +1743,310 @@
     <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="12" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="13" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="13" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="14" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="11" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="12" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1803,6 +2069,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff323232"/>
       <rgbColor rgb="ffadadad"/>
       <rgbColor rgb="ffd6d6d6"/>
@@ -1813,10 +2082,11 @@
       <rgbColor rgb="ffa6a29f"/>
       <rgbColor rgb="ffe3e3e3"/>
       <rgbColor rgb="fff4f9f8"/>
+      <rgbColor rgb="ffffea47"/>
       <rgbColor rgb="ffeecfb6"/>
-      <rgbColor rgb="fffebfc9"/>
       <rgbColor rgb="ffcff3e6"/>
       <rgbColor rgb="ffa4d4f3"/>
+      <rgbColor rgb="fffebfc9"/>
       <rgbColor rgb="fffefffe"/>
       <rgbColor rgb="ff94bee4"/>
       <rgbColor rgb="ff5e5e5e"/>
@@ -1835,14 +2105,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>27394</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>30569</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1064653</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>228636</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>556653</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>18451</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4946,7 +5216,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:P65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="4" width="33.6016" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" ht="50" customHeight="1">
+      <c r="B3" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="4"/>
+      <c r="C11" t="s" s="4">
+        <v>131</v>
+      </c>
+      <c r="D11" t="s" s="5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s" s="4">
+        <v>136</v>
+      </c>
+      <c r="D12" t="s" s="5">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="3">
+        <v>167</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s" s="4">
+        <v>168</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="4"/>
+      <c r="C15" t="s" s="4">
+        <v>191</v>
+      </c>
+      <c r="D15" t="s" s="5">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="4"/>
+      <c r="C16" t="s" s="4">
+        <v>200</v>
+      </c>
+      <c r="D16" t="s" s="5">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s" s="3">
+        <v>202</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s" s="4">
+        <v>200</v>
+      </c>
+      <c r="D18" t="s" s="5">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D10" location="'Sheet 1 - Table 1'!R2C1" tooltip="" display="Sheet 1 - Table 1"/>
+    <hyperlink ref="D11" location="'Sheet 1 - starry_ user inputs'!R2C1" tooltip="" display="Sheet 1 - starry_ user inputs"/>
+    <hyperlink ref="D12" location="'Sheet 1 - jaxoplanet implementa'!R2C1" tooltip="" display="Sheet 1 - jaxoplanet implementa"/>
+    <hyperlink ref="D14" location="'Sheet 2 - starry MathType'!R2C1" tooltip="" display="Sheet 2 - starry MathType"/>
+    <hyperlink ref="D15" location="'Sheet 2 - starry.math._get_cova'!R2C1" tooltip="" display="Sheet 2 - starry.math._get_cova"/>
+    <hyperlink ref="D16" location="'Sheet 2 - Drawings'!R1C1" tooltip="" display="Sheet 2 - Drawings"/>
+    <hyperlink ref="D18" location="'Sheet 3'!R1C1" tooltip="" display="Sheet 3"/>
+  </hyperlinks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A2:L52"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B4" xSplit="1" ySplit="3" activePane="bottomRight" state="frozen"/>
@@ -4954,1166 +5353,1608 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="23.2266" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="21.3672" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.0312" style="1" customWidth="1"/>
-    <col min="7" max="8" width="28.2734" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.0234" style="1" customWidth="1"/>
-    <col min="10" max="11" width="21.3672" style="1" customWidth="1"/>
-    <col min="12" max="16" width="16.3516" style="52" customWidth="1"/>
-    <col min="17" max="16384" width="16.3516" style="52" customWidth="1"/>
+    <col min="1" max="1" width="23.2266" style="6" customWidth="1"/>
+    <col min="2" max="2" width="28.5625" style="6" customWidth="1"/>
+    <col min="3" max="5" width="21.3672" style="6" customWidth="1"/>
+    <col min="6" max="6" width="37.0312" style="6" customWidth="1"/>
+    <col min="7" max="8" width="28.2734" style="6" customWidth="1"/>
+    <col min="9" max="10" width="24.0234" style="6" customWidth="1"/>
+    <col min="11" max="12" width="21.3672" style="6" customWidth="1"/>
+    <col min="13" max="16384" width="16.3516" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="A1" t="s" s="7">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" ht="71.05" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" t="s" s="7">
-        <v>3</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="A2" s="8"/>
+      <c r="B2" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" ht="71.05" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" t="s" s="11">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s" s="11">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s" s="11">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s" s="11">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s" s="11">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s" s="11">
+      <c r="A3" s="15"/>
+      <c r="B3" t="s" s="16">
         <v>10</v>
       </c>
-      <c r="I3" t="s" s="11">
+      <c r="C3" t="s" s="16">
         <v>11</v>
       </c>
-      <c r="J3" t="s" s="11">
+      <c r="D3" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="K3" t="s" s="12">
+      <c r="E3" t="s" s="16">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" ht="44.35" customHeight="1">
-      <c r="A4" t="s" s="13">
+      <c r="F3" t="s" s="16">
         <v>14</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="16"/>
+      <c r="G3" t="s" s="16">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s" s="16">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" ht="43.55" customHeight="1">
+      <c r="A4" t="s" s="18">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="19">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s" s="20">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s" s="20">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s" s="20">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s" s="20">
+        <v>26</v>
+      </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" t="s" s="20">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s" s="20">
+        <v>27</v>
+      </c>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" ht="43.55" customHeight="1">
-      <c r="A5" s="17"/>
-      <c r="B5" t="s" s="18">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s" s="19">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s" s="19">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s" s="19">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s" s="19">
-        <v>19</v>
-      </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" t="s" s="19">
-        <v>18</v>
-      </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="21"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" t="s" s="25">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s" s="25">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s" s="25">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s" s="25">
+        <v>30</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" t="s" s="25">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s" s="25">
+        <v>27</v>
+      </c>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
     </row>
     <row r="6" ht="43.55" customHeight="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="22"/>
-      <c r="C6" t="s" s="23">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s" s="23">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s" s="23">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s" s="23">
-        <v>22</v>
-      </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" t="s" s="23">
-        <v>23</v>
-      </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="25"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="28"/>
+      <c r="C6" t="s" s="29">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s" s="29">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s" s="29">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s" s="29">
+        <v>34</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" t="s" s="31">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s" s="31">
+        <v>35</v>
+      </c>
+      <c r="K6" s="30"/>
+      <c r="L6" s="32"/>
     </row>
     <row r="7" ht="43.55" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="26"/>
-      <c r="C7" t="s" s="19">
+      <c r="A7" s="23"/>
+      <c r="B7" t="s" s="33">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s" s="25">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s" s="25">
         <v>24</v>
       </c>
-      <c r="D7" t="s" s="19">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s" s="19">
+      <c r="E7" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s" s="25">
+        <v>39</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" t="s" s="34">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s" s="31">
+        <v>41</v>
+      </c>
+      <c r="K7" s="26"/>
+      <c r="L7" s="35"/>
+    </row>
+    <row r="8" ht="43.55" customHeight="1">
+      <c r="A8" s="23"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="30"/>
+      <c r="E8" t="s" s="29">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s" s="29">
+        <v>43</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" t="s" s="29">
+        <v>44</v>
+      </c>
+      <c r="J8" t="s" s="29">
+        <v>45</v>
+      </c>
+      <c r="K8" s="30"/>
+      <c r="L8" t="s" s="37">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" ht="43.55" customHeight="1">
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="26"/>
+      <c r="E9" t="s" s="25">
         <v>25</v>
       </c>
-      <c r="F7" t="s" s="19">
+      <c r="F9" t="s" s="25">
         <v>26</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
-    </row>
-    <row r="8" ht="43.55" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" t="s" s="27">
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" t="s" s="25">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s" s="25">
         <v>27</v>
       </c>
-      <c r="C8" t="s" s="23">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s" s="28">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s" s="28">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s" s="23">
-        <v>30</v>
-      </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="30"/>
-    </row>
-    <row r="9" ht="43.55" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="20"/>
-      <c r="E9" t="s" s="19">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s" s="19">
-        <v>32</v>
-      </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" t="s" s="19">
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
+    </row>
+    <row r="10" ht="43.55" customHeight="1">
+      <c r="A10" s="23"/>
+      <c r="B10" t="s" s="39">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" t="s" s="29">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s" s="29">
+        <v>50</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" t="s" s="29">
+        <v>51</v>
+      </c>
+      <c r="J10" t="s" s="29">
+        <v>52</v>
+      </c>
+      <c r="K10" s="30"/>
+      <c r="L10" s="32"/>
+    </row>
+    <row r="11" ht="43.55" customHeight="1">
+      <c r="A11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="26"/>
+      <c r="E11" t="s" s="25">
         <v>33</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" t="s" s="32">
+      <c r="F11" t="s" s="25">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" ht="43.55" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="24"/>
-      <c r="E10" t="s" s="23">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s" s="23">
-        <v>19</v>
-      </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" t="s" s="23">
-        <v>18</v>
-      </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="25"/>
-    </row>
-    <row r="11" ht="43.55" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" t="s" s="33">
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" t="s" s="31">
+        <v>33</v>
+      </c>
+      <c r="J11" t="s" s="31">
         <v>35</v>
       </c>
-      <c r="C11" t="s" s="19">
-        <v>36</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" t="s" s="19">
-        <v>37</v>
-      </c>
-      <c r="F11" t="s" s="19">
-        <v>38</v>
-      </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" t="s" s="19">
-        <v>39</v>
-      </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="27"/>
     </row>
     <row r="12" ht="43.55" customHeight="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="24"/>
-      <c r="E12" t="s" s="23">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s" s="23">
-        <v>26</v>
-      </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="30"/>
+      <c r="E12" t="s" s="29">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s" s="29">
+        <v>54</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" t="s" s="31">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s" s="31">
+        <v>35</v>
+      </c>
+      <c r="K12" s="30"/>
+      <c r="L12" s="32"/>
     </row>
     <row r="13" ht="43.55" customHeight="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="20"/>
-      <c r="E13" t="s" s="19">
-        <v>40</v>
-      </c>
-      <c r="F13" t="s" s="19">
-        <v>41</v>
-      </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="26"/>
+      <c r="E13" t="s" s="25">
+        <v>42</v>
+      </c>
+      <c r="F13" t="s" s="25">
+        <v>43</v>
+      </c>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" t="s" s="25">
+        <v>44</v>
+      </c>
+      <c r="J13" t="s" s="25">
+        <v>45</v>
+      </c>
+      <c r="K13" s="26"/>
+      <c r="L13" s="27"/>
     </row>
     <row r="14" ht="43.55" customHeight="1">
-      <c r="A14" s="17"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="24"/>
-      <c r="E14" t="s" s="23">
-        <v>31</v>
-      </c>
-      <c r="F14" t="s" s="23">
-        <v>32</v>
-      </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" t="s" s="23">
-        <v>33</v>
-      </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="25"/>
+      <c r="A14" s="23"/>
+      <c r="B14" t="s" s="40">
+        <v>56</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" t="s" s="29">
+        <v>55</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" t="s" s="31">
+        <v>55</v>
+      </c>
+      <c r="J14" t="s" s="31">
+        <v>35</v>
+      </c>
+      <c r="K14" s="30"/>
+      <c r="L14" s="32"/>
     </row>
     <row r="15" ht="43.55" customHeight="1">
-      <c r="A15" s="17"/>
-      <c r="B15" t="s" s="34">
-        <v>42</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" t="s" s="19">
-        <v>43</v>
-      </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" t="s" s="19">
-        <v>43</v>
-      </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="21"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="26"/>
+      <c r="D15" t="s" s="25">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s" s="25">
+        <v>58</v>
+      </c>
+      <c r="F15" s="26"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" t="s" s="31">
+        <v>59</v>
+      </c>
+      <c r="J15" t="s" s="31">
+        <v>60</v>
+      </c>
+      <c r="K15" s="26"/>
+      <c r="L15" t="s" s="41">
+        <v>61</v>
+      </c>
     </row>
     <row r="16" ht="43.55" customHeight="1">
-      <c r="A16" s="17"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="24"/>
-      <c r="D16" t="s" s="23">
-        <v>44</v>
-      </c>
-      <c r="E16" t="s" s="23">
-        <v>45</v>
-      </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" t="s" s="35">
-        <v>46</v>
-      </c>
+      <c r="A16" s="23"/>
+      <c r="B16" t="s" s="42">
+        <v>62</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" t="s" s="29">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s" s="29">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s" s="29">
+        <v>65</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" t="s" s="29">
+        <v>66</v>
+      </c>
+      <c r="L16" s="32"/>
     </row>
     <row r="17" ht="43.55" customHeight="1">
-      <c r="A17" s="17"/>
-      <c r="B17" t="s" s="18">
-        <v>47</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" t="s" s="19">
-        <v>48</v>
-      </c>
-      <c r="E17" t="s" s="19">
-        <v>49</v>
-      </c>
-      <c r="F17" t="s" s="19">
-        <v>50</v>
-      </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" t="s" s="19">
-        <v>51</v>
-      </c>
-      <c r="K17" s="21"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" t="s" s="25">
+        <v>67</v>
+      </c>
+      <c r="G17" t="s" s="25">
+        <v>68</v>
+      </c>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="27"/>
     </row>
     <row r="18" ht="43.55" customHeight="1">
-      <c r="A18" s="17"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" t="s" s="23">
-        <v>52</v>
-      </c>
-      <c r="G18" t="s" s="23">
-        <v>53</v>
-      </c>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="25"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" t="s" s="29">
+        <v>69</v>
+      </c>
+      <c r="G18" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="H18" s="36"/>
+      <c r="I18" t="s" s="29">
+        <v>71</v>
+      </c>
+      <c r="J18" s="30"/>
+      <c r="K18" t="s" s="29">
+        <v>72</v>
+      </c>
+      <c r="L18" s="32"/>
     </row>
     <row r="19" ht="43.55" customHeight="1">
-      <c r="A19" s="17"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" t="s" s="19">
-        <v>54</v>
-      </c>
-      <c r="G19" t="s" s="19">
-        <v>55</v>
-      </c>
-      <c r="H19" s="31"/>
-      <c r="I19" t="s" s="19">
-        <v>56</v>
-      </c>
-      <c r="J19" t="s" s="19">
-        <v>57</v>
-      </c>
-      <c r="K19" s="21"/>
+      <c r="A19" s="23"/>
+      <c r="B19" t="s" s="43">
+        <v>73</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" t="s" s="25">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s" s="25">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s" s="25">
+        <v>76</v>
+      </c>
+      <c r="G19" s="26"/>
+      <c r="H19" t="s" s="25">
+        <v>77</v>
+      </c>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" t="s" s="25">
+        <v>78</v>
+      </c>
+      <c r="L19" s="27"/>
     </row>
     <row r="20" ht="43.55" customHeight="1">
-      <c r="A20" s="17"/>
-      <c r="B20" t="s" s="36">
-        <v>58</v>
-      </c>
-      <c r="C20" s="24"/>
-      <c r="D20" t="s" s="23">
-        <v>59</v>
-      </c>
-      <c r="E20" t="s" s="23">
-        <v>60</v>
-      </c>
-      <c r="F20" t="s" s="23">
-        <v>61</v>
-      </c>
-      <c r="G20" s="24"/>
-      <c r="H20" t="s" s="23">
-        <v>62</v>
-      </c>
-      <c r="I20" s="24"/>
-      <c r="J20" t="s" s="23">
-        <v>63</v>
-      </c>
-      <c r="K20" s="25"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" t="s" s="29">
+        <v>65</v>
+      </c>
+      <c r="G20" s="30"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="32"/>
     </row>
     <row r="21" ht="43.55" customHeight="1">
-      <c r="A21" s="17"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" t="s" s="19">
-        <v>50</v>
-      </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="21"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" t="s" s="25">
+        <v>79</v>
+      </c>
+      <c r="G21" t="s" s="44">
+        <v>80</v>
+      </c>
+      <c r="H21" s="38"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" t="s" s="25">
+        <v>81</v>
+      </c>
+      <c r="L21" s="27"/>
     </row>
     <row r="22" ht="43.55" customHeight="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" t="s" s="23">
-        <v>64</v>
-      </c>
-      <c r="G22" t="s" s="37">
-        <v>65</v>
-      </c>
-      <c r="H22" s="29"/>
-      <c r="I22" s="24"/>
-      <c r="J22" t="s" s="23">
-        <v>66</v>
-      </c>
-      <c r="K22" s="25"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" t="s" s="45">
+        <v>82</v>
+      </c>
+      <c r="H22" s="36"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="32"/>
     </row>
     <row r="23" ht="43.55" customHeight="1">
-      <c r="A23" s="17"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" t="s" s="38">
-        <v>67</v>
-      </c>
-      <c r="H23" s="31"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="21"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" t="s" s="25">
+        <v>83</v>
+      </c>
+      <c r="G23" t="s" s="46">
+        <v>84</v>
+      </c>
+      <c r="H23" s="38"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="27"/>
     </row>
     <row r="24" ht="43.55" customHeight="1">
-      <c r="A24" s="17"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" t="s" s="23">
-        <v>68</v>
-      </c>
-      <c r="G24" t="s" s="39">
-        <v>69</v>
-      </c>
-      <c r="H24" s="29"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="25"/>
-    </row>
-    <row r="25" ht="43.55" customHeight="1">
-      <c r="A25" s="17"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" t="s" s="38">
-        <v>67</v>
-      </c>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="21"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" t="s" s="45">
+        <v>82</v>
+      </c>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="32"/>
+    </row>
+    <row r="25" ht="122.05" customHeight="1">
+      <c r="A25" s="23"/>
+      <c r="B25" t="s" s="43">
+        <v>85</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" t="s" s="25">
+        <v>86</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" t="s" s="25">
+        <v>87</v>
+      </c>
+      <c r="L25" s="27"/>
     </row>
     <row r="26" ht="122.05" customHeight="1">
-      <c r="A26" s="17"/>
-      <c r="B26" t="s" s="18">
-        <v>70</v>
-      </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="20"/>
-      <c r="E26" t="s" s="19">
-        <v>71</v>
-      </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" t="s" s="23">
-        <v>72</v>
-      </c>
-      <c r="K26" s="25"/>
+      <c r="A26" s="23"/>
+      <c r="B26" t="s" s="43">
+        <v>88</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="26"/>
+      <c r="E26" t="s" s="25">
+        <v>89</v>
+      </c>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" t="s" s="29">
+        <v>90</v>
+      </c>
+      <c r="L26" s="32"/>
     </row>
     <row r="27" ht="122.05" customHeight="1">
-      <c r="A27" s="17"/>
-      <c r="B27" t="s" s="18">
-        <v>73</v>
-      </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" t="s" s="19">
-        <v>74</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" t="s" s="19">
-        <v>75</v>
-      </c>
-      <c r="K27" s="21"/>
-    </row>
-    <row r="28" ht="122.05" customHeight="1">
-      <c r="A28" s="17"/>
-      <c r="B28" t="s" s="18">
-        <v>76</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" t="s" s="19">
-        <v>77</v>
-      </c>
-      <c r="E28" t="s" s="19">
-        <v>78</v>
-      </c>
-      <c r="F28" t="s" s="23">
-        <v>79</v>
-      </c>
-      <c r="G28" t="s" s="28">
-        <v>80</v>
-      </c>
-      <c r="H28" t="s" s="23">
-        <v>81</v>
-      </c>
-      <c r="I28" s="24"/>
-      <c r="J28" t="s" s="23">
-        <v>82</v>
-      </c>
-      <c r="K28" s="25"/>
+      <c r="A27" s="23"/>
+      <c r="B27" t="s" s="43">
+        <v>91</v>
+      </c>
+      <c r="C27" s="26"/>
+      <c r="D27" t="s" s="25">
+        <v>92</v>
+      </c>
+      <c r="E27" t="s" s="25">
+        <v>93</v>
+      </c>
+      <c r="F27" t="s" s="25">
+        <v>94</v>
+      </c>
+      <c r="G27" t="s" s="47">
+        <v>95</v>
+      </c>
+      <c r="H27" t="s" s="25">
+        <v>96</v>
+      </c>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" t="s" s="25">
+        <v>97</v>
+      </c>
+      <c r="L27" s="27"/>
+    </row>
+    <row r="28" ht="69.7" customHeight="1">
+      <c r="A28" s="23"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" t="s" s="29">
+        <v>98</v>
+      </c>
+      <c r="G28" s="30"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="32"/>
     </row>
     <row r="29" ht="69.7" customHeight="1">
-      <c r="A29" s="17"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" t="s" s="19">
-        <v>83</v>
-      </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="21"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" t="s" s="25">
+        <v>99</v>
+      </c>
+      <c r="G29" t="s" s="25">
+        <v>100</v>
+      </c>
+      <c r="H29" s="38"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="27"/>
     </row>
     <row r="30" ht="69.7" customHeight="1">
-      <c r="A30" s="17"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" t="s" s="23">
-        <v>84</v>
-      </c>
-      <c r="G30" t="s" s="23">
-        <v>85</v>
-      </c>
-      <c r="H30" s="29"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="25"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" t="s" s="29">
+        <v>101</v>
+      </c>
+      <c r="G30" t="s" s="29">
+        <v>102</v>
+      </c>
+      <c r="H30" s="36"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="32"/>
     </row>
     <row r="31" ht="69.7" customHeight="1">
-      <c r="A31" s="17"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" t="s" s="19">
-        <v>86</v>
-      </c>
-      <c r="G31" t="s" s="19">
-        <v>87</v>
-      </c>
-      <c r="H31" s="31"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="21"/>
-    </row>
-    <row r="32" ht="69.7" customHeight="1">
-      <c r="A32" s="17"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" t="s" s="23">
-        <v>88</v>
-      </c>
-      <c r="G32" t="s" s="23">
-        <v>85</v>
-      </c>
-      <c r="H32" s="29"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="25"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" t="s" s="25">
+        <v>103</v>
+      </c>
+      <c r="G31" t="s" s="25">
+        <v>100</v>
+      </c>
+      <c r="H31" s="38"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="27"/>
+    </row>
+    <row r="32" ht="43.55" customHeight="1">
+      <c r="A32" s="23"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" t="s" s="29">
+        <v>104</v>
+      </c>
+      <c r="G32" t="s" s="29">
+        <v>102</v>
+      </c>
+      <c r="H32" s="36"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="32"/>
     </row>
     <row r="33" ht="43.55" customHeight="1">
-      <c r="A33" s="17"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" t="s" s="19">
-        <v>89</v>
-      </c>
-      <c r="G33" t="s" s="19">
-        <v>87</v>
-      </c>
-      <c r="H33" s="31"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="21"/>
-    </row>
-    <row r="34" ht="43.55" customHeight="1">
-      <c r="A34" s="17"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" t="s" s="23">
-        <v>90</v>
-      </c>
-      <c r="G34" s="24"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="25"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" t="s" s="25">
+        <v>105</v>
+      </c>
+      <c r="G33" s="26"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="27"/>
+    </row>
+    <row r="34" ht="95.9" customHeight="1">
+      <c r="A34" s="23"/>
+      <c r="B34" t="s" s="48">
+        <v>106</v>
+      </c>
+      <c r="C34" s="49"/>
+      <c r="D34" t="s" s="50">
+        <v>107</v>
+      </c>
+      <c r="E34" t="s" s="50">
+        <v>108</v>
+      </c>
+      <c r="F34" t="s" s="29">
+        <v>109</v>
+      </c>
+      <c r="G34" s="30"/>
+      <c r="H34" t="s" s="29">
+        <v>110</v>
+      </c>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="32"/>
     </row>
     <row r="35" ht="95.9" customHeight="1">
-      <c r="A35" s="17"/>
-      <c r="B35" t="s" s="40">
-        <v>91</v>
-      </c>
-      <c r="C35" s="41"/>
-      <c r="D35" t="s" s="42">
-        <v>92</v>
-      </c>
-      <c r="E35" t="s" s="42">
-        <v>93</v>
-      </c>
-      <c r="F35" t="s" s="19">
-        <v>94</v>
-      </c>
-      <c r="G35" s="20"/>
-      <c r="H35" t="s" s="19">
-        <v>95</v>
-      </c>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="21"/>
-    </row>
-    <row r="36" ht="95.9" customHeight="1">
-      <c r="A36" s="17"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" t="s" s="23">
-        <v>96</v>
-      </c>
-      <c r="G36" t="s" s="23">
-        <v>97</v>
-      </c>
-      <c r="H36" s="29"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="25"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" t="s" s="25">
+        <v>111</v>
+      </c>
+      <c r="G35" t="s" s="25">
+        <v>112</v>
+      </c>
+      <c r="H35" s="38"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="27"/>
+    </row>
+    <row r="36" ht="122.05" customHeight="1">
+      <c r="A36" t="s" s="51">
+        <v>113</v>
+      </c>
+      <c r="B36" s="52"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" t="s" s="29">
+        <v>114</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="32"/>
     </row>
     <row r="37" ht="122.05" customHeight="1">
-      <c r="A37" t="s" s="43">
-        <v>98</v>
-      </c>
-      <c r="B37" s="44"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" t="s" s="19">
-        <v>99</v>
-      </c>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="21"/>
-    </row>
-    <row r="38" ht="122.05" customHeight="1">
-      <c r="A38" s="17"/>
-      <c r="B38" t="s" s="36">
-        <v>100</v>
-      </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" t="s" s="23">
-        <v>101</v>
-      </c>
-      <c r="F38" t="s" s="23">
-        <v>102</v>
-      </c>
-      <c r="G38" t="s" s="23">
-        <v>103</v>
-      </c>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" t="s" s="23">
-        <v>104</v>
-      </c>
-      <c r="K38" s="25"/>
-    </row>
-    <row r="39" ht="43.55" customHeight="1">
-      <c r="A39" s="17"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" t="s" s="19">
-        <v>105</v>
-      </c>
-      <c r="G39" t="s" s="19">
-        <v>97</v>
-      </c>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="21"/>
-    </row>
-    <row r="40" ht="69.7" customHeight="1">
-      <c r="A40" s="17"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" t="s" s="23">
-        <v>106</v>
-      </c>
-      <c r="G40" t="s" s="23">
-        <v>107</v>
-      </c>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="25"/>
-    </row>
-    <row r="41" ht="43.55" customHeight="1">
-      <c r="A41" s="17"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" t="s" s="19">
-        <v>108</v>
-      </c>
-      <c r="G41" t="s" s="19">
-        <v>109</v>
-      </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="21"/>
-    </row>
-    <row r="42" ht="69.7" customHeight="1">
-      <c r="A42" s="17"/>
-      <c r="B42" t="s" s="36">
-        <v>110</v>
-      </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" t="s" s="23">
-        <v>111</v>
-      </c>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" t="s" s="23">
+      <c r="A37" s="23"/>
+      <c r="B37" t="s" s="43">
+        <v>115</v>
+      </c>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" t="s" s="25">
+        <v>116</v>
+      </c>
+      <c r="F37" t="s" s="25">
+        <v>117</v>
+      </c>
+      <c r="G37" t="s" s="25">
+        <v>118</v>
+      </c>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" t="s" s="25">
+        <v>119</v>
+      </c>
+      <c r="L37" s="27"/>
+    </row>
+    <row r="38" ht="43.55" customHeight="1">
+      <c r="A38" s="23"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" t="s" s="29">
+        <v>120</v>
+      </c>
+      <c r="G38" t="s" s="29">
         <v>112</v>
       </c>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="25"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="32"/>
+    </row>
+    <row r="39" ht="69.7" customHeight="1">
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" t="s" s="25">
+        <v>121</v>
+      </c>
+      <c r="G39" t="s" s="25">
+        <v>122</v>
+      </c>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="27"/>
+    </row>
+    <row r="40" ht="43.55" customHeight="1">
+      <c r="A40" s="23"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" t="s" s="29">
+        <v>123</v>
+      </c>
+      <c r="G40" t="s" s="29">
+        <v>124</v>
+      </c>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="32"/>
+    </row>
+    <row r="41" ht="69.7" customHeight="1">
+      <c r="A41" s="23"/>
+      <c r="B41" t="s" s="43">
+        <v>125</v>
+      </c>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" t="s" s="25">
+        <v>126</v>
+      </c>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" t="s" s="25">
+        <v>127</v>
+      </c>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="27"/>
+    </row>
+    <row r="42" ht="43.55" customHeight="1">
+      <c r="A42" s="23"/>
+      <c r="B42" t="s" s="42">
+        <v>128</v>
+      </c>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" t="s" s="29">
+        <v>129</v>
+      </c>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
+      <c r="L42" s="32"/>
     </row>
     <row r="43" ht="43.55" customHeight="1">
-      <c r="A43" s="17"/>
-      <c r="B43" t="s" s="18">
-        <v>113</v>
-      </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" t="s" s="19">
-        <v>114</v>
-      </c>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="21"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="27"/>
     </row>
     <row r="44" ht="43.55" customHeight="1">
-      <c r="A44" s="45"/>
-      <c r="B44" s="46"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="25"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
+      <c r="L44" s="32"/>
     </row>
     <row r="45" ht="43.55" customHeight="1">
-      <c r="A45" s="45"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="21"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="27"/>
     </row>
     <row r="46" ht="43.55" customHeight="1">
-      <c r="A46" s="45"/>
-      <c r="B46" s="46"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="25"/>
+      <c r="A46" s="53"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="32"/>
     </row>
     <row r="47" ht="43.55" customHeight="1">
-      <c r="A47" s="45"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="21"/>
+      <c r="A47" t="s" s="55">
+        <v>130</v>
+      </c>
+      <c r="B47" s="54"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="27"/>
     </row>
     <row r="48" ht="43.55" customHeight="1">
-      <c r="A48" t="s" s="47">
-        <v>115</v>
-      </c>
-      <c r="B48" s="46"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="25"/>
+      <c r="A48" s="53"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
+      <c r="L48" s="32"/>
     </row>
     <row r="49" ht="43.55" customHeight="1">
-      <c r="A49" s="45"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-      <c r="K49" s="21"/>
+      <c r="A49" s="53"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="27"/>
     </row>
     <row r="50" ht="43.55" customHeight="1">
-      <c r="A50" s="45"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24"/>
-      <c r="K50" s="25"/>
+      <c r="A50" s="53"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
+      <c r="K50" s="30"/>
+      <c r="L50" s="32"/>
     </row>
     <row r="51" ht="43.55" customHeight="1">
-      <c r="A51" s="45"/>
-      <c r="B51" s="44"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="21"/>
-    </row>
-    <row r="52" ht="43.55" customHeight="1">
-      <c r="A52" s="45"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="25"/>
-    </row>
-    <row r="53" ht="44.1" customHeight="1">
-      <c r="A53" s="48"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="50"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="50"/>
-      <c r="H53" s="50"/>
-      <c r="I53" s="50"/>
-      <c r="J53" s="50"/>
-      <c r="K53" s="51"/>
-    </row>
-    <row r="55" ht="35.45" customHeight="1">
-      <c r="L55" t="s" s="53">
-        <v>116</v>
-      </c>
-      <c r="M55" s="53"/>
-      <c r="N55" s="53"/>
-      <c r="O55" s="53"/>
-      <c r="P55" s="53"/>
-    </row>
-    <row r="56" ht="24.45" customHeight="1">
-      <c r="L56" t="s" s="54">
-        <v>117</v>
-      </c>
-      <c r="M56" t="s" s="55">
-        <v>118</v>
-      </c>
-      <c r="N56" t="s" s="55">
-        <v>119</v>
-      </c>
-      <c r="O56" s="56"/>
-      <c r="P56" s="57"/>
-    </row>
-    <row r="57" ht="23.25" customHeight="1">
-      <c r="L57" s="58"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
-      <c r="P57" s="16"/>
-    </row>
-    <row r="58" ht="22.85" customHeight="1">
-      <c r="L58" s="59"/>
-      <c r="M58" s="20"/>
-      <c r="N58" s="20"/>
-      <c r="O58" s="20"/>
-      <c r="P58" s="21"/>
-    </row>
-    <row r="59" ht="22.85" customHeight="1">
-      <c r="L59" s="60"/>
-      <c r="M59" s="24"/>
-      <c r="N59" s="24"/>
-      <c r="O59" s="24"/>
-      <c r="P59" s="25"/>
-    </row>
-    <row r="60" ht="22.85" customHeight="1">
-      <c r="L60" s="59"/>
-      <c r="M60" s="20"/>
-      <c r="N60" s="20"/>
-      <c r="O60" s="20"/>
-      <c r="P60" s="21"/>
-    </row>
-    <row r="61" ht="22.85" customHeight="1">
-      <c r="L61" s="60"/>
-      <c r="M61" s="24"/>
-      <c r="N61" s="24"/>
-      <c r="O61" s="24"/>
-      <c r="P61" s="25"/>
-    </row>
-    <row r="62" ht="22.85" customHeight="1">
-      <c r="L62" s="59"/>
-      <c r="M62" s="20"/>
-      <c r="N62" s="20"/>
-      <c r="O62" s="20"/>
-      <c r="P62" s="21"/>
-    </row>
-    <row r="63" ht="22.85" customHeight="1">
-      <c r="L63" s="60"/>
-      <c r="M63" s="24"/>
-      <c r="N63" s="24"/>
-      <c r="O63" s="24"/>
-      <c r="P63" s="25"/>
-    </row>
-    <row r="64" ht="22.85" customHeight="1">
-      <c r="L64" s="59"/>
-      <c r="M64" s="20"/>
-      <c r="N64" s="20"/>
-      <c r="O64" s="20"/>
-      <c r="P64" s="21"/>
-    </row>
-    <row r="65" ht="23.1" customHeight="1">
-      <c r="L65" s="61"/>
-      <c r="M65" s="62"/>
-      <c r="N65" s="62"/>
-      <c r="O65" s="62"/>
-      <c r="P65" s="63"/>
+      <c r="A51" s="53"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="27"/>
+    </row>
+    <row r="52" ht="44.1" customHeight="1">
+      <c r="A52" s="56"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="58"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="I52" s="58"/>
+      <c r="J52" s="58"/>
+      <c r="K52" s="58"/>
+      <c r="L52" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="E28:E34"/>
-    <mergeCell ref="J28:J34"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D28:D34"/>
-    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B27:B33"/>
+    <mergeCell ref="E27:E33"/>
+    <mergeCell ref="K27:K33"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D27:D33"/>
+    <mergeCell ref="D16:D18"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="A4:A36"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="A4:A35"/>
     <mergeCell ref="D2:H2"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="E20:E25"/>
-    <mergeCell ref="H28:H34"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="L55:P55"/>
+    <mergeCell ref="H19:H23"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="D19:D24"/>
+    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="H27:H33"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="A36:A42"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" location="" tooltip="" display="A1"/>
-    <hyperlink ref="I5" r:id="rId2" location="" tooltip="" display="A1"/>
-    <hyperlink ref="E6" r:id="rId3" location="" tooltip="" display="A2"/>
-    <hyperlink ref="I6" r:id="rId4" location="" tooltip="" display="A2_inv"/>
-    <hyperlink ref="E7" r:id="rId5" location="" tooltip="" display="A"/>
-    <hyperlink ref="E8" r:id="rId6" location="" tooltip="" display="rT"/>
-    <hyperlink ref="E9" r:id="rId7" location="" tooltip="" display="R"/>
-    <hyperlink ref="I9" r:id="rId8" location="" tooltip="" display="R_full"/>
-    <hyperlink ref="K9" r:id="rId9" location="" tooltip="" display="collado1989"/>
-    <hyperlink ref="E10" r:id="rId10" location="" tooltip="" display="A1"/>
-    <hyperlink ref="I10" r:id="rId11" location="" tooltip="" display="A1"/>
-    <hyperlink ref="E11" r:id="rId12" location="" tooltip="" display="sT"/>
-    <hyperlink ref="I11" r:id="rId13" location="" tooltip="" display="solution_vector"/>
-    <hyperlink ref="E12" r:id="rId14" location="" tooltip="" display="A"/>
-    <hyperlink ref="E13" r:id="rId15" location="" tooltip="" display="tensordotRz"/>
-    <hyperlink ref="E14" r:id="rId16" location="" tooltip="" display="R"/>
-    <hyperlink ref="I14" r:id="rId17" location="" tooltip="" display="R_full"/>
-    <hyperlink ref="E15" r:id="rId18" location="" tooltip="" display="dotR"/>
-    <hyperlink ref="I15" r:id="rId19" location="" tooltip="" display="dotR"/>
-    <hyperlink ref="E16" r:id="rId20" location="" tooltip="" display="core.OpsYlm.right_project"/>
-    <hyperlink ref="K16" r:id="rId21" location="" tooltip="" display="starry tutorial: basic"/>
-    <hyperlink ref="E17" r:id="rId22" location="" tooltip="" display="core.OpsLD.flux"/>
-    <hyperlink ref="F17" r:id="rId23" location="" tooltip="" display="compute the occultation mask"/>
-    <hyperlink ref="F18" r:id="rId24" location="" tooltip="" display="get the Agol `c` coefficients"/>
-    <hyperlink ref="G18" r:id="rId25" location="" tooltip="" display="get_cl.cc"/>
-    <hyperlink ref="F19" r:id="rId26" location="" tooltip="" display="compute the occultation flux"/>
-    <hyperlink ref="G19" r:id="rId27" location="" tooltip="" display="limbdark.cc"/>
-    <hyperlink ref="I19" r:id="rId28" location="" tooltip="" display="light_curve"/>
-    <hyperlink ref="E20" r:id="rId29" location="" tooltip="" display="core.OpsYlm.X"/>
-    <hyperlink ref="F20" r:id="rId30" location="" tooltip="" display="determine the shape of X"/>
-    <hyperlink ref="F21" r:id="rId31" location="" tooltip="" display="compute the occultation mask"/>
-    <hyperlink ref="F22" r:id="rId32" location="" tooltip="" display="update X according to rotational operator"/>
-    <hyperlink ref="F24" r:id="rId33" location="" tooltip="" display="update X according to (rotation + occultation operator)"/>
-    <hyperlink ref="E26" r:id="rId34" location="" tooltip="" display="core.OpsOblate.X"/>
-    <hyperlink ref="E27" r:id="rId35" location="" tooltip="" display="core.OpsReflected.X"/>
-    <hyperlink ref="E28" r:id="rId36" location="" tooltip="" display="core.OpsSystem.X"/>
-    <hyperlink ref="F28" r:id="rId37" location="" tooltip="" display="get relative positions of the system"/>
-    <hyperlink ref="F29" r:id="rId38" location="" tooltip="" display="get rotational phases (theta)"/>
-    <hyperlink ref="F30" r:id="rId39" location="" tooltip="" display="get phase curve of the primary object"/>
-    <hyperlink ref="F31" r:id="rId40" location="" tooltip="" display="get phase curve of the secondary object"/>
-    <hyperlink ref="F32" r:id="rId41" location="" tooltip="" display="get occultation for the primary object (transit)"/>
-    <hyperlink ref="F33" r:id="rId42" location="" tooltip="" display="get occultation for the second object"/>
-    <hyperlink ref="F34" r:id="rId43" location="" tooltip="" display="construct the design matrix"/>
-    <hyperlink ref="E35" r:id="rId44" location="" tooltip="" display="System.flux"/>
-    <hyperlink ref="F35" r:id="rId45" location="" tooltip="" display="get weighted ylm coefficients"/>
-    <hyperlink ref="F36" r:id="rId46" location="" tooltip="" display="calculate light curve"/>
-    <hyperlink ref="E37" r:id="rId47" location="" tooltip="" display="System.set_data"/>
-    <hyperlink ref="E38" r:id="rId48" location="" tooltip="" display="System.solve"/>
-    <hyperlink ref="G41" r:id="rId49" location="" tooltip="" display="LinAlgType.solve"/>
-    <hyperlink ref="E42" r:id="rId50" location="" tooltip="" display="System.lnlike"/>
+    <hyperlink ref="E4" r:id="rId1" location="" tooltip="" display="A1"/>
+    <hyperlink ref="I4" r:id="rId2" location="" tooltip="" display="A1"/>
+    <hyperlink ref="E5" r:id="rId3" location="" tooltip="" display="A2"/>
+    <hyperlink ref="I5" r:id="rId4" location="" tooltip="" display="A2_inv"/>
+    <hyperlink ref="E6" r:id="rId5" location="" tooltip="" display="A"/>
+    <hyperlink ref="I6" r:id="rId6" location="" tooltip="" display="A"/>
+    <hyperlink ref="E7" r:id="rId7" location="" tooltip="" display="rT"/>
+    <hyperlink ref="I7" r:id="rId8" location="" tooltip="" display="rT_solution_vector"/>
+    <hyperlink ref="E8" r:id="rId9" location="" tooltip="" display="R"/>
+    <hyperlink ref="I8" r:id="rId10" location="" tooltip="" display="R_full"/>
+    <hyperlink ref="L8" r:id="rId11" location="" tooltip="" display="collado1989"/>
+    <hyperlink ref="E9" r:id="rId12" location="" tooltip="" display="A1"/>
+    <hyperlink ref="I9" r:id="rId13" location="" tooltip="" display="A1"/>
+    <hyperlink ref="E10" r:id="rId14" location="" tooltip="" display="sT"/>
+    <hyperlink ref="I10" r:id="rId15" location="" tooltip="" display="solution_vector"/>
+    <hyperlink ref="E11" r:id="rId16" location="" tooltip="" display="A"/>
+    <hyperlink ref="I11" r:id="rId17" location="" tooltip="" display="A"/>
+    <hyperlink ref="E12" r:id="rId18" location="" tooltip="" display="tensordotRz"/>
+    <hyperlink ref="I12" r:id="rId19" location="" tooltip="" display="dotR"/>
+    <hyperlink ref="E13" r:id="rId20" location="" tooltip="" display="R"/>
+    <hyperlink ref="I13" r:id="rId21" location="" tooltip="" display="R_full"/>
+    <hyperlink ref="E14" r:id="rId22" location="" tooltip="" display="dotR"/>
+    <hyperlink ref="I14" r:id="rId23" location="" tooltip="" display="dotR"/>
+    <hyperlink ref="E15" r:id="rId24" location="" tooltip="" display="core.OpsYlm.right_project"/>
+    <hyperlink ref="I15" r:id="rId25" location="" tooltip="" display="right_project"/>
+    <hyperlink ref="L15" r:id="rId26" location="" tooltip="" display="starry tutorial: basic"/>
+    <hyperlink ref="E16" r:id="rId27" location="" tooltip="" display="core.OpsLD.flux"/>
+    <hyperlink ref="F16" r:id="rId28" location="" tooltip="" display="compute the occultation mask"/>
+    <hyperlink ref="F17" r:id="rId29" location="" tooltip="" display="get the Agol `c` coefficients"/>
+    <hyperlink ref="G17" r:id="rId30" location="" tooltip="" display="get_cl.cc"/>
+    <hyperlink ref="F18" r:id="rId31" location="" tooltip="" display="compute the occultation flux"/>
+    <hyperlink ref="G18" r:id="rId32" location="" tooltip="" display="limbdark.cc"/>
+    <hyperlink ref="I18" r:id="rId33" location="" tooltip="" display="light_curve"/>
+    <hyperlink ref="E19" r:id="rId34" location="" tooltip="" display="core.OpsYlm.X"/>
+    <hyperlink ref="F19" r:id="rId35" location="" tooltip="" display="determine the shape of X"/>
+    <hyperlink ref="F20" r:id="rId36" location="" tooltip="" display="compute the occultation mask"/>
+    <hyperlink ref="F21" r:id="rId37" location="" tooltip="" display="update X according to rotational operator"/>
+    <hyperlink ref="F23" r:id="rId38" location="" tooltip="" display="update X according to (rotation + occultation operator)"/>
+    <hyperlink ref="E25" r:id="rId39" location="" tooltip="" display="core.OpsOblate.X"/>
+    <hyperlink ref="E26" r:id="rId40" location="" tooltip="" display="core.OpsReflected.X"/>
+    <hyperlink ref="E27" r:id="rId41" location="" tooltip="" display="core.OpsSystem.X"/>
+    <hyperlink ref="F27" r:id="rId42" location="" tooltip="" display="get relative positions of the system"/>
+    <hyperlink ref="F28" r:id="rId43" location="" tooltip="" display="get rotational phases (theta)"/>
+    <hyperlink ref="F29" r:id="rId44" location="" tooltip="" display="get phase curve of the primary object"/>
+    <hyperlink ref="F30" r:id="rId45" location="" tooltip="" display="get phase curve of the secondary object"/>
+    <hyperlink ref="F31" r:id="rId46" location="" tooltip="" display="get occultation for the primary object (transit)"/>
+    <hyperlink ref="F32" r:id="rId47" location="" tooltip="" display="get occultation for the second object"/>
+    <hyperlink ref="F33" r:id="rId48" location="" tooltip="" display="construct the design matrix"/>
+    <hyperlink ref="E34" r:id="rId49" location="" tooltip="" display="System.flux"/>
+    <hyperlink ref="F34" r:id="rId50" location="" tooltip="" display="get weighted ylm coefficients"/>
+    <hyperlink ref="F35" r:id="rId51" location="" tooltip="" display="calculate light curve"/>
+    <hyperlink ref="E36" r:id="rId52" location="" tooltip="" display="System.set_data"/>
+    <hyperlink ref="E37" r:id="rId53" location="" tooltip="" display="System.solve"/>
+    <hyperlink ref="G40" r:id="rId54" location="" tooltip="" display="LinAlgType.solve"/>
+    <hyperlink ref="E41" r:id="rId55" location="" tooltip="" display="System.lnlike"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId51"/>
-  <legacyDrawing r:id="rId52"/>
+  <drawing r:id="rId56"/>
+  <legacyDrawing r:id="rId57"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A2:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="60" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="60" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="35.45" customHeight="1">
+      <c r="A1" t="s" s="61">
+        <v>131</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+    </row>
+    <row r="2" ht="24.45" customHeight="1">
+      <c r="A2" t="s" s="62">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s" s="63">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s" s="63">
+        <v>135</v>
+      </c>
+      <c r="D2" s="64"/>
+      <c r="E2" s="65"/>
+    </row>
+    <row r="3" ht="23.25" customHeight="1">
+      <c r="A3" s="66"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" ht="22.85" customHeight="1">
+      <c r="A4" s="67"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+    </row>
+    <row r="5" ht="22.85" customHeight="1">
+      <c r="A5" s="68"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" ht="22.85" customHeight="1">
+      <c r="A6" s="67"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" ht="22.85" customHeight="1">
+      <c r="A7" s="68"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" ht="22.85" customHeight="1">
+      <c r="A8" s="67"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" ht="22.85" customHeight="1">
+      <c r="A9" s="68"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" ht="22.85" customHeight="1">
+      <c r="A10" s="67"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
+    </row>
+    <row r="11" ht="23.1" customHeight="1">
+      <c r="A11" s="69"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A2:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="A4" xSplit="0" ySplit="3" activePane="bottomLeft" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="4" width="16.3516" style="70" customWidth="1"/>
+    <col min="5" max="6" width="21.0469" style="70" customWidth="1"/>
+    <col min="7" max="7" width="23.5547" style="70" customWidth="1"/>
+    <col min="8" max="8" width="25.5312" style="70" customWidth="1"/>
+    <col min="9" max="9" width="28.2031" style="70" customWidth="1"/>
+    <col min="10" max="13" width="21.5938" style="70" customWidth="1"/>
+    <col min="14" max="16384" width="16.3516" style="70" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="35.45" customHeight="1">
+      <c r="A1" t="s" s="61">
+        <v>136</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+    </row>
+    <row r="2" ht="24.1" customHeight="1">
+      <c r="A2" t="s" s="71">
+        <v>138</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" t="s" s="72">
+        <v>139</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" t="s" s="73">
+        <v>140</v>
+      </c>
+      <c r="L2" s="10"/>
+      <c r="M2" s="74"/>
+    </row>
+    <row r="3" ht="56.2" customHeight="1">
+      <c r="A3" t="s" s="75">
+        <v>141</v>
+      </c>
+      <c r="B3" t="s" s="16">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s" s="16">
+        <v>143</v>
+      </c>
+      <c r="D3" t="s" s="16">
+        <v>144</v>
+      </c>
+      <c r="E3" t="s" s="16">
+        <v>145</v>
+      </c>
+      <c r="F3" t="s" s="16">
+        <v>146</v>
+      </c>
+      <c r="G3" t="s" s="16">
+        <v>147</v>
+      </c>
+      <c r="H3" t="s" s="16">
+        <v>148</v>
+      </c>
+      <c r="I3" t="s" s="16">
+        <v>149</v>
+      </c>
+      <c r="J3" t="s" s="16">
+        <v>150</v>
+      </c>
+      <c r="K3" t="s" s="16">
+        <v>151</v>
+      </c>
+      <c r="L3" t="s" s="16">
+        <v>152</v>
+      </c>
+      <c r="M3" t="s" s="17">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" ht="23.25" customHeight="1">
+      <c r="A4" t="s" s="76">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s" s="20">
+        <v>155</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" t="s" s="77">
+        <v>156</v>
+      </c>
+      <c r="G4" t="s" s="20">
+        <v>155</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" t="s" s="78">
+        <v>157</v>
+      </c>
+      <c r="L4" t="s" s="20">
+        <v>155</v>
+      </c>
+      <c r="M4" s="22"/>
+    </row>
+    <row r="5" ht="22.85" customHeight="1">
+      <c r="A5" t="s" s="79">
+        <v>158</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" t="s" s="45">
+        <v>159</v>
+      </c>
+      <c r="G5" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="H5" s="26"/>
+      <c r="I5" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="J5" s="26"/>
+      <c r="K5" t="s" s="46">
+        <v>160</v>
+      </c>
+      <c r="L5" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="M5" t="s" s="41">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" ht="22.85" customHeight="1">
+      <c r="A6" t="s" s="79">
+        <v>161</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" t="s" s="29">
+        <v>155</v>
+      </c>
+      <c r="D6" t="s" s="29">
+        <v>155</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" t="s" s="45">
+        <v>162</v>
+      </c>
+      <c r="G6" t="s" s="29">
+        <v>155</v>
+      </c>
+      <c r="H6" t="s" s="29">
+        <v>155</v>
+      </c>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="32"/>
+    </row>
+    <row r="7" ht="22.85" customHeight="1">
+      <c r="A7" t="s" s="79">
+        <v>163</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="D7" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="E7" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="F7" t="s" s="45">
+        <v>164</v>
+      </c>
+      <c r="G7" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="H7" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="I7" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="27"/>
+    </row>
+    <row r="8" ht="22.85" customHeight="1">
+      <c r="A8" s="68"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" t="s" s="45">
+        <v>165</v>
+      </c>
+      <c r="G8" t="s" s="29">
+        <v>155</v>
+      </c>
+      <c r="H8" t="s" s="29">
+        <v>155</v>
+      </c>
+      <c r="I8" s="30"/>
+      <c r="J8" t="s" s="29">
+        <v>155</v>
+      </c>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="32"/>
+    </row>
+    <row r="9" ht="22.85" customHeight="1">
+      <c r="A9" s="67"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" t="s" s="45">
+        <v>166</v>
+      </c>
+      <c r="G9" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="H9" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="I9" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="J9" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+    </row>
+    <row r="10" ht="22.85" customHeight="1">
+      <c r="A10" s="68"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="32"/>
+    </row>
+    <row r="11" ht="22.85" customHeight="1">
+      <c r="A11" s="67"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+    </row>
+    <row r="12" ht="22.85" customHeight="1">
+      <c r="A12" s="68"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="32"/>
+    </row>
+    <row r="13" ht="23.1" customHeight="1">
+      <c r="A13" s="80"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="82"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J23"/>
+  <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -6121,273 +6962,321 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="64" customWidth="1"/>
-    <col min="2" max="2" width="20.7031" style="64" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="64" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="89" customWidth="1"/>
-    <col min="7" max="7" width="19.6641" style="89" customWidth="1"/>
-    <col min="8" max="10" width="16.3516" style="89" customWidth="1"/>
-    <col min="11" max="16384" width="16.3516" style="89" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="83" customWidth="1"/>
+    <col min="2" max="2" width="20.7031" style="83" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="83" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="83" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="A1" t="s" s="7">
+        <v>168</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="65">
-        <v>120</v>
-      </c>
-      <c r="B2" t="s" s="66">
-        <v>121</v>
-      </c>
-      <c r="C2" t="s" s="66">
-        <v>122</v>
-      </c>
-      <c r="D2" t="s" s="66">
-        <v>12</v>
-      </c>
-      <c r="E2" s="67"/>
+      <c r="A2" t="s" s="84">
+        <v>168</v>
+      </c>
+      <c r="B2" t="s" s="85">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s" s="85">
+        <v>171</v>
+      </c>
+      <c r="D2" t="s" s="85">
+        <v>19</v>
+      </c>
+      <c r="E2" s="86"/>
     </row>
     <row r="3" ht="20.3" customHeight="1">
-      <c r="A3" t="s" s="68">
-        <v>123</v>
-      </c>
-      <c r="B3" t="s" s="69">
-        <v>124</v>
-      </c>
-      <c r="C3" t="s" s="70">
-        <v>125</v>
-      </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="72"/>
+      <c r="A3" t="s" s="87">
+        <v>172</v>
+      </c>
+      <c r="B3" t="s" s="88">
+        <v>173</v>
+      </c>
+      <c r="C3" t="s" s="89">
+        <v>174</v>
+      </c>
+      <c r="D3" s="90"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" ht="19.95" customHeight="1">
-      <c r="A4" t="s" s="73">
-        <v>126</v>
-      </c>
-      <c r="B4" t="s" s="74">
-        <v>127</v>
-      </c>
-      <c r="C4" t="s" s="75">
-        <v>125</v>
-      </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="76"/>
+      <c r="A4" t="s" s="92">
+        <v>175</v>
+      </c>
+      <c r="B4" t="s" s="93">
+        <v>176</v>
+      </c>
+      <c r="C4" t="s" s="94">
+        <v>174</v>
+      </c>
+      <c r="D4" s="38"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" ht="31.95" customHeight="1">
-      <c r="A5" t="s" s="73">
-        <v>128</v>
-      </c>
-      <c r="B5" t="s" s="77">
-        <v>129</v>
-      </c>
-      <c r="C5" t="s" s="78">
-        <v>125</v>
-      </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
+      <c r="A5" t="s" s="92">
+        <v>177</v>
+      </c>
+      <c r="B5" t="s" s="95">
+        <v>178</v>
+      </c>
+      <c r="C5" t="s" s="96">
+        <v>174</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="97"/>
     </row>
     <row r="6" ht="19.95" customHeight="1">
-      <c r="A6" t="s" s="73">
-        <v>130</v>
-      </c>
-      <c r="B6" t="s" s="74">
-        <v>131</v>
-      </c>
-      <c r="C6" t="s" s="75">
-        <v>125</v>
-      </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="76"/>
+      <c r="A6" t="s" s="92">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s" s="93">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s" s="94">
+        <v>174</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="35"/>
     </row>
     <row r="7" ht="19.95" customHeight="1">
-      <c r="A7" t="s" s="73">
-        <v>132</v>
-      </c>
-      <c r="B7" t="s" s="77">
-        <v>133</v>
-      </c>
-      <c r="C7" t="s" s="78">
-        <v>125</v>
-      </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
+      <c r="A7" t="s" s="92">
+        <v>181</v>
+      </c>
+      <c r="B7" t="s" s="95">
+        <v>182</v>
+      </c>
+      <c r="C7" t="s" s="96">
+        <v>174</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="97"/>
     </row>
     <row r="8" ht="19.95" customHeight="1">
-      <c r="A8" t="s" s="79">
-        <v>134</v>
-      </c>
-      <c r="B8" t="s" s="80">
-        <v>135</v>
-      </c>
-      <c r="C8" t="s" s="81">
-        <v>136</v>
-      </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="83"/>
+      <c r="A8" t="s" s="98">
+        <v>183</v>
+      </c>
+      <c r="B8" t="s" s="99">
+        <v>184</v>
+      </c>
+      <c r="C8" t="s" s="100">
+        <v>185</v>
+      </c>
+      <c r="D8" s="101"/>
+      <c r="E8" s="102"/>
     </row>
     <row r="9" ht="19.95" customHeight="1">
-      <c r="A9" t="s" s="73">
-        <v>137</v>
-      </c>
-      <c r="B9" t="s" s="77">
-        <v>133</v>
-      </c>
-      <c r="C9" t="s" s="78">
-        <v>125</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
+      <c r="A9" t="s" s="92">
+        <v>186</v>
+      </c>
+      <c r="B9" t="s" s="95">
+        <v>182</v>
+      </c>
+      <c r="C9" t="s" s="96">
+        <v>174</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="97"/>
     </row>
     <row r="10" ht="19.95" customHeight="1">
-      <c r="A10" t="s" s="73">
-        <v>138</v>
-      </c>
-      <c r="B10" t="s" s="74">
-        <v>139</v>
-      </c>
-      <c r="C10" t="s" s="75">
-        <v>125</v>
-      </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="76"/>
+      <c r="A10" t="s" s="92">
+        <v>187</v>
+      </c>
+      <c r="B10" t="s" s="93">
+        <v>188</v>
+      </c>
+      <c r="C10" t="s" s="94">
+        <v>174</v>
+      </c>
+      <c r="D10" s="38"/>
+      <c r="E10" s="35"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" t="s" s="84">
-        <v>140</v>
-      </c>
-      <c r="B11" t="s" s="85">
-        <v>141</v>
-      </c>
-      <c r="C11" t="s" s="86">
-        <v>125</v>
-      </c>
-      <c r="D11" s="87"/>
-      <c r="E11" s="88"/>
-    </row>
-    <row r="13" ht="27.65" customHeight="1">
-      <c r="F13" t="s" s="2">
-        <v>142</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" ht="20.55" customHeight="1">
-      <c r="F14" t="s" s="65">
-        <v>143</v>
-      </c>
-      <c r="G14" t="s" s="66">
-        <v>121</v>
-      </c>
-      <c r="H14" t="s" s="66">
-        <v>122</v>
-      </c>
-      <c r="I14" t="s" s="66">
-        <v>144</v>
-      </c>
-      <c r="J14" s="67"/>
-    </row>
-    <row r="15" ht="56.3" customHeight="1">
-      <c r="F15" t="s" s="68">
-        <v>145</v>
-      </c>
-      <c r="G15" t="s" s="69">
-        <v>146</v>
-      </c>
-      <c r="H15" t="s" s="70">
-        <v>125</v>
-      </c>
-      <c r="I15" t="s" s="70">
-        <v>147</v>
-      </c>
-      <c r="J15" s="72"/>
-    </row>
-    <row r="16" ht="31.95" customHeight="1">
-      <c r="F16" t="s" s="73">
-        <v>148</v>
-      </c>
-      <c r="G16" t="s" s="74">
-        <v>149</v>
-      </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="76"/>
-    </row>
-    <row r="17" ht="19.95" customHeight="1">
-      <c r="F17" s="17"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30"/>
-    </row>
-    <row r="18" ht="19.95" customHeight="1">
-      <c r="F18" s="17"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="76"/>
-    </row>
-    <row r="19" ht="19.95" customHeight="1">
-      <c r="F19" s="17"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="30"/>
-    </row>
-    <row r="20" ht="19.95" customHeight="1">
-      <c r="F20" s="17"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="76"/>
-    </row>
-    <row r="21" ht="19.95" customHeight="1">
-      <c r="F21" s="17"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="30"/>
-    </row>
-    <row r="22" ht="19.95" customHeight="1">
-      <c r="F22" s="17"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="76"/>
-    </row>
-    <row r="23" ht="20.2" customHeight="1">
-      <c r="F23" s="90"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="88"/>
+      <c r="A11" t="s" s="103">
+        <v>189</v>
+      </c>
+      <c r="B11" t="s" s="104">
+        <v>190</v>
+      </c>
+      <c r="C11" t="s" s="105">
+        <v>174</v>
+      </c>
+      <c r="D11" s="106"/>
+      <c r="E11" s="107"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F13:J13"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16.3516" style="108" customWidth="1"/>
+    <col min="2" max="2" width="19.6641" style="108" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="108" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="108" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="7">
+        <v>191</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="A2" t="s" s="84">
+        <v>193</v>
+      </c>
+      <c r="B2" t="s" s="85">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s" s="85">
+        <v>171</v>
+      </c>
+      <c r="D2" t="s" s="85">
+        <v>194</v>
+      </c>
+      <c r="E2" s="86"/>
+    </row>
+    <row r="3" ht="56.3" customHeight="1">
+      <c r="A3" t="s" s="87">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s" s="88">
+        <v>196</v>
+      </c>
+      <c r="C3" t="s" s="89">
+        <v>174</v>
+      </c>
+      <c r="D3" t="s" s="89">
+        <v>197</v>
+      </c>
+      <c r="E3" s="91"/>
+    </row>
+    <row r="4" ht="31.95" customHeight="1">
+      <c r="A4" t="s" s="92">
+        <v>198</v>
+      </c>
+      <c r="B4" t="s" s="93">
+        <v>199</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="35"/>
+    </row>
+    <row r="5" ht="19.95" customHeight="1">
+      <c r="A5" s="23"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="97"/>
+    </row>
+    <row r="6" ht="19.95" customHeight="1">
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="35"/>
+    </row>
+    <row r="7" ht="19.95" customHeight="1">
+      <c r="A7" s="23"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="97"/>
+    </row>
+    <row r="8" ht="19.95" customHeight="1">
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="35"/>
+    </row>
+    <row r="9" ht="19.95" customHeight="1">
+      <c r="A9" s="23"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="97"/>
+    </row>
+    <row r="10" ht="19.95" customHeight="1">
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="35"/>
+    </row>
+    <row r="11" ht="20.2" customHeight="1">
+      <c r="A11" s="109"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="107"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I15" r:id="rId1" location="" tooltip="" display="theano.tensor.slinalg"/>
+    <hyperlink ref="D3" r:id="rId1" location="" tooltip="" display="theano.tensor.slinalg"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="16384" width="10" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>